<commit_message>
updated test courseload list
</commit_message>
<xml_diff>
--- a/Faculty Courseloads 20-21.xlsx
+++ b/Faculty Courseloads 20-21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panda/Desktop/Automate forms project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817E2CA8-F53E-6348-A87F-9386F318E780}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F2E16F-0BB4-C84D-A03E-4ACAF4E8BAF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22160" yWindow="5740" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6200" yWindow="10720" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lecturers" sheetId="1" r:id="rId1"/>
@@ -247,48 +247,6 @@
     <t xml:space="preserve">3 courses 60% </t>
   </si>
   <si>
-    <t xml:space="preserve">3 ER 6 </t>
-  </si>
-  <si>
-    <t>2 IC 2</t>
-  </si>
-  <si>
-    <t>2 UP 1</t>
-  </si>
-  <si>
-    <t>1 TU 3D, 1 UT 3</t>
-  </si>
-  <si>
-    <t>2 IO 5W</t>
-  </si>
-  <si>
-    <t>2 BC 2</t>
-  </si>
-  <si>
-    <t>3 YA 3D</t>
-  </si>
-  <si>
-    <t>3 FR 5W</t>
-  </si>
-  <si>
-    <t>2 PA 100W</t>
-  </si>
-  <si>
-    <t>1 UK 5W; 1 JKLH 21W</t>
-  </si>
-  <si>
-    <t>2 BA 3</t>
-  </si>
-  <si>
-    <t>2 EKP 3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 EIC 131A</t>
-  </si>
-  <si>
-    <t>2 EF 4</t>
-  </si>
-  <si>
     <t>Heron, Cady</t>
   </si>
   <si>
@@ -305,6 +263,48 @@
   </si>
   <si>
     <t>Leigh, Damian</t>
+  </si>
+  <si>
+    <t>2 EF 10A</t>
+  </si>
+  <si>
+    <t>3 FR 101</t>
+  </si>
+  <si>
+    <t>2 PA 102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 ER 10A </t>
+  </si>
+  <si>
+    <t>1 UK 10A; 1 JKLH 101</t>
+  </si>
+  <si>
+    <t>2 IC 102</t>
+  </si>
+  <si>
+    <t>2 UP 102</t>
+  </si>
+  <si>
+    <t>1 TU 10A, 1 UT 101</t>
+  </si>
+  <si>
+    <t>2 BC 102</t>
+  </si>
+  <si>
+    <t>2 PK 101</t>
+  </si>
+  <si>
+    <t>2 EKP 10A</t>
+  </si>
+  <si>
+    <t>2 BA 101</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 EIC 102</t>
+  </si>
+  <si>
+    <t>2 jk 101</t>
   </si>
 </sst>
 </file>
@@ -935,7 +935,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="93" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <selection pane="topRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -989,13 +989,13 @@
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>27</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="4" spans="1:8" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>9</v>
@@ -1025,19 +1025,19 @@
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="23"/>
@@ -1057,19 +1057,19 @@
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="23"/>
@@ -1077,19 +1077,19 @@
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="23"/>
@@ -1097,17 +1097,17 @@
     </row>
     <row r="9" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>14</v>

</xml_diff>